<commit_message>
Delete city and wallet and bank change added
</commit_message>
<xml_diff>
--- a/extra deatil/IMT Hub Initial Data Upload.xlsx
+++ b/extra deatil/IMT Hub Initial Data Upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nabeel.jamil\Downloads\imrh\extra deatil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C933CE56-EA37-41C0-B6CD-9809BC6498F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1E395E-6BAA-402B-B341-D14B3A683C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="103">
   <si>
     <t>ISO 2 Char</t>
   </si>
@@ -479,7 +479,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -498,6 +498,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -511,7 +517,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -527,6 +533,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,8 +816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F940D0E-E75E-4A56-AAF4-E27BEE2B7AF5}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -836,19 +843,13 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D3" t="s">
         <v>83</v>
@@ -856,14 +857,22 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
         <v>52</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="9" t="s">
         <v>55</v>
       </c>
     </row>
@@ -917,7 +926,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -966,9 +975,12 @@
       <c r="C18" s="4" t="s">
         <v>74</v>
       </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" s="9" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1017,9 +1029,12 @@
       <c r="C25" s="4" t="s">
         <v>73</v>
       </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="A27" s="9" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1068,9 +1083,12 @@
       <c r="C32" s="4" t="s">
         <v>81</v>
       </c>
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="A34" s="9" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IMT find by added
</commit_message>
<xml_diff>
--- a/extra deatil/IMT Hub Initial Data Upload.xlsx
+++ b/extra deatil/IMT Hub Initial Data Upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nabeel.jamil\Downloads\imrh\extra deatil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1E395E-6BAA-402B-B341-D14B3A683C9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A5F7A3-CB03-407B-B249-3333ABFE4032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <author>Nabeel Ahmed Jamil</author>
   </authors>
   <commentList>
-    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{110C0565-BFE4-4B1C-822A-36FEABB4B4CA}">
+    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{110C0565-BFE4-4B1C-822A-36FEABB4B4CA}">
       <text>
         <r>
           <rPr>
@@ -66,7 +66,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C10" authorId="0" shapeId="0" xr:uid="{A9C73575-6580-44E5-95D8-92B5CF5D9DDC}">
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{A9C73575-6580-44E5-95D8-92B5CF5D9DDC}">
       <text>
         <r>
           <rPr>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{B70927CF-71BF-4C11-AC89-A6A56CB85862}">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{B70927CF-71BF-4C11-AC89-A6A56CB85862}">
       <text>
         <r>
           <rPr>
@@ -115,12 +115,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="C48" authorId="0" shapeId="0" xr:uid="{4A756318-A337-43D3-AB49-5EB37DC950E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nabeel Ahmed Jamil:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+this api user when user click on the add button to like the new country with partner</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="120">
   <si>
     <t>ISO 2 Char</t>
   </si>
@@ -290,15 +314,6 @@
     <t>Api Detail for Country</t>
   </si>
   <si>
-    <t>Fetch All Country City</t>
-  </si>
-  <si>
-    <t>Fetch All Country Bank</t>
-  </si>
-  <si>
-    <t>Fetch All Country Wallets</t>
-  </si>
-  <si>
     <t>Api Detail for City</t>
   </si>
   <si>
@@ -413,9 +428,6 @@
     <t>Api Status</t>
   </si>
   <si>
-    <t>if partner detai it will auto delete the (ref table detail)</t>
-  </si>
-  <si>
     <t>Not Realtie</t>
   </si>
   <si>
@@ -429,13 +441,76 @@
   </si>
   <si>
     <t>15975365484</t>
+  </si>
+  <si>
+    <t>if partner detai it will auto delete the (partner_country, partner_city, partner_wallet, partner_bank)</t>
+  </si>
+  <si>
+    <t>Api Detail for MTO Countries</t>
+  </si>
+  <si>
+    <t>Fetch All Link Country with Mito Partner</t>
+  </si>
+  <si>
+    <t>Note :- we check if mto countrie like with the same mto partner then send error msg</t>
+  </si>
+  <si>
+    <t>Delete Mto Country</t>
+  </si>
+  <si>
+    <t>Add Mto Countrie</t>
+  </si>
+  <si>
+    <t>delete only from partner_country table</t>
+  </si>
+  <si>
+    <t>Api Detail for Mto City</t>
+  </si>
+  <si>
+    <t>Api Detail for Mto Wallet</t>
+  </si>
+  <si>
+    <t>Api Detail for Mto Bank</t>
+  </si>
+  <si>
+    <t>Api Detail for Mto Product</t>
+  </si>
+  <si>
+    <t>Find By City Id</t>
+  </si>
+  <si>
+    <t>Find By Bank Id</t>
+  </si>
+  <si>
+    <t>api call to fetch the single result of bank, call when edit button click</t>
+  </si>
+  <si>
+    <t>api call to fetch the single result of city, call when edit button click</t>
+  </si>
+  <si>
+    <t>Find Product By Id</t>
+  </si>
+  <si>
+    <t>api call to fetch the single reuslt of product, call when edit button click</t>
+  </si>
+  <si>
+    <t>Find By Wallet Id</t>
+  </si>
+  <si>
+    <t>api call to fetch the single result of wallet, call when edit button click</t>
+  </si>
+  <si>
+    <t>Find By MTO Partner Id</t>
+  </si>
+  <si>
+    <t>api call to fetch the single reuslt of mto partner, call when edit button click</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -477,6 +552,19 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -814,32 +902,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F940D0E-E75E-4A56-AAF4-E27BEE2B7AF5}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="83" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -852,7 +940,7 @@
         <v>50</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -860,264 +948,373 @@
         <v>51</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>52</v>
       </c>
-      <c r="D5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="D6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D7" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
-        <v>59</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+      <c r="A14" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D14" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>82</v>
+        <v>87</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D16" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>74</v>
+        <v>110</v>
+      </c>
+      <c r="C18" t="s">
+        <v>113</v>
       </c>
       <c r="D18" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>69</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" t="s">
-        <v>83</v>
+      <c r="A22" s="9" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>70</v>
+        <v>88</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D23" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" t="s">
+        <v>112</v>
+      </c>
+      <c r="D26" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>76</v>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>77</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B30" t="s">
-        <v>78</v>
-      </c>
-      <c r="D30" t="s">
-        <v>83</v>
+      <c r="A30" s="9" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
-        <v>79</v>
+        <v>89</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D31" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C32" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D36" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D32" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+      <c r="C43" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B38" t="s">
-        <v>88</v>
-      </c>
-      <c r="C38" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>89</v>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>104</v>
+      </c>
+      <c r="C49" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1726,7 +1923,7 @@
         <v>35</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1746,13 +1943,13 @@
         <v>3.94</v>
       </c>
       <c r="G3" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H3" t="s">
         <v>35</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1775,10 +1972,10 @@
         <v>38</v>
       </c>
       <c r="H4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J4" t="s">
         <v>49</v>

</xml_diff>

<commit_message>
Mto Partern detail added
</commit_message>
<xml_diff>
--- a/extra deatil/IMT Hub Initial Data Upload.xlsx
+++ b/extra deatil/IMT Hub Initial Data Upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nabeel.jamil\Downloads\imrh\extra deatil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0912C9-D01F-41BC-9F6C-96BA66BD7593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306AF801-0947-4353-8FF7-C89B8BCAA57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C48" authorId="0" shapeId="0" xr:uid="{4A756318-A337-43D3-AB49-5EB37DC950E6}">
+    <comment ref="C51" authorId="0" shapeId="0" xr:uid="{4A756318-A337-43D3-AB49-5EB37DC950E6}">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="126">
   <si>
     <t>ISO 2 Char</t>
   </si>
@@ -443,9 +443,6 @@
     <t>15975365484</t>
   </si>
   <si>
-    <t>if partner detai it will auto delete the (partner_country, partner_city, partner_wallet, partner_bank)</t>
-  </si>
-  <si>
     <t>Api Detail for MTO Countries</t>
   </si>
   <si>
@@ -522,6 +519,9 @@
   </si>
   <si>
     <t>TOGGLE, 3</t>
+  </si>
+  <si>
+    <t>if partner detai it will auto delete the (partner_country, partner_city, partner_wallet, partner_bank,partner_country_product)</t>
   </si>
 </sst>
 </file>
@@ -920,17 +920,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F940D0E-E75E-4A56-AAF4-E27BEE2B7AF5}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="83" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="111.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -971,10 +971,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C5" t="s">
         <v>114</v>
-      </c>
-      <c r="C5" t="s">
-        <v>115</v>
       </c>
       <c r="D5" t="s">
         <v>80</v>
@@ -1049,7 +1049,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>65</v>
@@ -1060,10 +1060,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>79</v>
+        <v>87</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D16" t="s">
         <v>80</v>
@@ -1071,7 +1071,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D17" t="s">
         <v>80</v>
@@ -1079,10 +1082,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>110</v>
-      </c>
-      <c r="C18" t="s">
-        <v>113</v>
+        <v>62</v>
       </c>
       <c r="D18" t="s">
         <v>80</v>
@@ -1090,7 +1090,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>63</v>
+        <v>109</v>
+      </c>
+      <c r="C19" t="s">
+        <v>112</v>
       </c>
       <c r="D19" t="s">
         <v>80</v>
@@ -1098,37 +1101,34 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
         <v>64</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C21" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="D21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="9" t="s">
         <v>72</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D23" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>79</v>
+        <v>54</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D24" t="s">
         <v>80</v>
@@ -1136,7 +1136,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>67</v>
+        <v>88</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D25" t="s">
         <v>80</v>
@@ -1144,10 +1147,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>111</v>
-      </c>
-      <c r="C26" t="s">
-        <v>112</v>
+        <v>66</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D26" t="s">
         <v>80</v>
@@ -1155,7 +1158,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D27" t="s">
         <v>80</v>
@@ -1163,45 +1166,45 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
+        <v>110</v>
+      </c>
+      <c r="C28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C30" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B31" t="s">
-        <v>89</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B32" t="s">
-        <v>74</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>75</v>
+        <v>54</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D33" t="s">
         <v>80</v>
@@ -1209,10 +1212,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>116</v>
-      </c>
-      <c r="C34" t="s">
-        <v>117</v>
+        <v>89</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D34" t="s">
         <v>80</v>
@@ -1220,7 +1223,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>76</v>
+        <v>74</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D35" t="s">
         <v>80</v>
@@ -1228,111 +1234,153 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D36" t="s">
         <v>80</v>
       </c>
     </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>115</v>
+      </c>
+      <c r="C37" t="s">
+        <v>116</v>
+      </c>
+      <c r="D37" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>81</v>
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D38" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>82</v>
+        <v>77</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="D39" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B40" t="s">
-        <v>83</v>
-      </c>
-    </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
-        <v>118</v>
-      </c>
-      <c r="C41" t="s">
-        <v>119</v>
+      <c r="A41" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>84</v>
+        <v>82</v>
+      </c>
+      <c r="D42" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>85</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>99</v>
+        <v>83</v>
+      </c>
+      <c r="D43" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>86</v>
+        <v>117</v>
+      </c>
+      <c r="C44" t="s">
+        <v>118</v>
+      </c>
+      <c r="D44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="9" t="s">
-        <v>100</v>
+      <c r="B46" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D46" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
-        <v>54</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>65</v>
+        <v>86</v>
+      </c>
+      <c r="D47" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B49" t="s">
-        <v>104</v>
-      </c>
-      <c r="C49" t="s">
-        <v>102</v>
+      <c r="A49" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
         <v>103</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C52" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>102</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>108</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1574,28 +1622,28 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s">
         <v>120</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>121</v>
-      </c>
-      <c r="C8" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1643,28 +1691,28 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" t="s">
         <v>120</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>121</v>
-      </c>
-      <c r="C7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
partner sub service added
</commit_message>
<xml_diff>
--- a/extra deatil/IMT Hub Initial Data Upload.xlsx
+++ b/extra deatil/IMT Hub Initial Data Upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nabeel.jamil\Downloads\imrh\extra deatil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{306AF801-0947-4353-8FF7-C89B8BCAA57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFEF2C4-28C2-4065-B62D-AD06FB6EA978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,7 +115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C51" authorId="0" shapeId="0" xr:uid="{4A756318-A337-43D3-AB49-5EB37DC950E6}">
+    <comment ref="C46" authorId="0" shapeId="0" xr:uid="{4A756318-A337-43D3-AB49-5EB37DC950E6}">
       <text>
         <r>
           <rPr>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="137">
   <si>
     <t>ISO 2 Char</t>
   </si>
@@ -449,18 +449,12 @@
     <t>Fetch All Link Country with Mito Partner</t>
   </si>
   <si>
-    <t>Note :- we check if mto countrie like with the same mto partner then send error msg</t>
-  </si>
-  <si>
     <t>Delete Mto Country</t>
   </si>
   <si>
     <t>Add Mto Countrie</t>
   </si>
   <si>
-    <t>delete only from partner_country table</t>
-  </si>
-  <si>
     <t>Api Detail for Mto City</t>
   </si>
   <si>
@@ -470,9 +464,6 @@
     <t>Api Detail for Mto Bank</t>
   </si>
   <si>
-    <t>Api Detail for Mto Product</t>
-  </si>
-  <si>
     <t>Find By City Id</t>
   </si>
   <si>
@@ -522,6 +513,48 @@
   </si>
   <si>
     <t>if partner detai it will auto delete the (partner_country, partner_city, partner_wallet, partner_bank,partner_country_product)</t>
+  </si>
+  <si>
+    <t>delete only from partner_country table with partenr id and country id</t>
+  </si>
+  <si>
+    <t>Add Mto City</t>
+  </si>
+  <si>
+    <t>Delete Mto City</t>
+  </si>
+  <si>
+    <t>Note :- we check if mto city link with the same mto partner then send error msg</t>
+  </si>
+  <si>
+    <t>Note :- we check if mto countrie link with the same mto partner then send error msg</t>
+  </si>
+  <si>
+    <t>Note :- we check if mto wallet link with the same mto partner then send error msg</t>
+  </si>
+  <si>
+    <t>Note :- we check if mto bank like with the same mto partner then send error msg</t>
+  </si>
+  <si>
+    <t>delete only from partner_cityt able with partenr id and city id</t>
+  </si>
+  <si>
+    <t>Add Mto Wallet</t>
+  </si>
+  <si>
+    <t>Delete Mto Wallet</t>
+  </si>
+  <si>
+    <t>delete only from partner_wallet table with partenr id and city id</t>
+  </si>
+  <si>
+    <t>Add Mto Bank</t>
+  </si>
+  <si>
+    <t>Delete Mto Bank</t>
+  </si>
+  <si>
+    <t>delete only from partner_bank table with partenr id and bank id</t>
   </si>
 </sst>
 </file>
@@ -920,10 +953,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F940D0E-E75E-4A56-AAF4-E27BEE2B7AF5}">
-  <dimension ref="A1:D61"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C65" sqref="C65"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,10 +1004,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
         <v>80</v>
@@ -1042,14 +1075,25 @@
         <v>80</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
-        <v>56</v>
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>65</v>
@@ -1060,10 +1104,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>65</v>
+        <v>60</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D16" t="s">
         <v>80</v>
@@ -1071,10 +1115,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D17" t="s">
         <v>80</v>
@@ -1082,7 +1123,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>62</v>
+        <v>106</v>
+      </c>
+      <c r="C18" t="s">
+        <v>109</v>
       </c>
       <c r="D18" t="s">
         <v>80</v>
@@ -1090,10 +1134,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>109</v>
-      </c>
-      <c r="C19" t="s">
-        <v>112</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
         <v>80</v>
@@ -1101,34 +1142,48 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>63</v>
+        <v>64</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>71</v>
       </c>
       <c r="D20" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>64</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="A21" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
-        <v>72</v>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>54</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>79</v>
       </c>
       <c r="D24" t="s">
         <v>80</v>
@@ -1136,10 +1191,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>88</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D25" t="s">
         <v>80</v>
@@ -1147,10 +1199,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>79</v>
+        <v>107</v>
+      </c>
+      <c r="C26" t="s">
+        <v>108</v>
       </c>
       <c r="D26" t="s">
         <v>80</v>
@@ -1158,7 +1210,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D27" t="s">
         <v>80</v>
@@ -1166,45 +1218,56 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>110</v>
-      </c>
-      <c r="C28" t="s">
-        <v>111</v>
+        <v>69</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="D28" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D29" t="s">
-        <v>80</v>
+      <c r="A29" s="9" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>69</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>70</v>
+        <v>54</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D30" t="s">
         <v>80</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>89</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>73</v>
+      <c r="B32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D32" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
         <v>80</v>
@@ -1212,10 +1275,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>89</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>65</v>
+        <v>112</v>
+      </c>
+      <c r="C34" t="s">
+        <v>113</v>
       </c>
       <c r="D34" t="s">
         <v>80</v>
@@ -1223,10 +1286,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>74</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D35" t="s">
         <v>80</v>
@@ -1234,26 +1294,23 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>75</v>
+        <v>77</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="D36" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>115</v>
-      </c>
-      <c r="C37" t="s">
-        <v>116</v>
-      </c>
-      <c r="D37" t="s">
-        <v>80</v>
+      <c r="A37" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
         <v>80</v>
@@ -1261,23 +1318,37 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D39" t="s">
         <v>80</v>
       </c>
     </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" t="s">
+        <v>115</v>
+      </c>
+      <c r="D40" t="s">
+        <v>80</v>
+      </c>
+    </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
-        <v>81</v>
+      <c r="B41" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>82</v>
+        <v>85</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="D42" t="s">
         <v>80</v>
@@ -1285,26 +1356,20 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D43" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>117</v>
-      </c>
-      <c r="C44" t="s">
-        <v>118</v>
-      </c>
-      <c r="D44" t="s">
-        <v>80</v>
+      <c r="A44" s="9" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="D45" t="s">
         <v>80</v>
@@ -1312,10 +1377,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>85</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>125</v>
+        <v>54</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D46" t="s">
         <v>80</v>
@@ -1323,65 +1388,109 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>86</v>
+        <v>102</v>
+      </c>
+      <c r="C47" t="s">
+        <v>127</v>
       </c>
       <c r="D47" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="9" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D48" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+        <v>124</v>
+      </c>
+      <c r="C50" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
-        <v>103</v>
-      </c>
-      <c r="C52" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+        <v>125</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>102</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+        <v>131</v>
+      </c>
+      <c r="C53" t="s">
+        <v>128</v>
+      </c>
+      <c r="D53" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>132</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
-        <v>108</v>
-      </c>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" t="s">
+        <v>129</v>
+      </c>
+      <c r="D56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>135</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="D57" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C60" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1622,28 +1731,28 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B8" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1691,28 +1800,28 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B7" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mto city, bank, wallet fetch added base on partner id and country code
</commit_message>
<xml_diff>
--- a/extra deatil/IMT Hub Initial Data Upload.xlsx
+++ b/extra deatil/IMT Hub Initial Data Upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nabeel.jamil\Downloads\imrh\extra deatil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFEF2C4-28C2-4065-B62D-AD06FB6EA978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CD58B5-EC25-4B1F-B855-4CF1213BBA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="140">
   <si>
     <t>ISO 2 Char</t>
   </si>
@@ -555,6 +555,15 @@
   </si>
   <si>
     <t>delete only from partner_bank table with partenr id and bank id</t>
+  </si>
+  <si>
+    <t>Done in city contrller</t>
+  </si>
+  <si>
+    <t>Fetch All Link Wallet with Mito Partner</t>
+  </si>
+  <si>
+    <t>Fetch All Link Bank with Mito Partner</t>
   </si>
 </sst>
 </file>
@@ -953,10 +962,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F940D0E-E75E-4A56-AAF4-E27BEE2B7AF5}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1415,64 +1424,58 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>124</v>
-      </c>
-      <c r="C50" t="s">
-        <v>126</v>
-      </c>
-      <c r="D50" t="s">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>125</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>130</v>
+        <v>87</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>137</v>
       </c>
       <c r="D51" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>104</v>
+      <c r="B52" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D52" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>131</v>
-      </c>
-      <c r="C53" t="s">
-        <v>128</v>
+        <v>125</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="D53" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
-        <v>132</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D54" t="s">
-        <v>80</v>
+      <c r="A54" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>105</v>
+      <c r="B55" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
-        <v>134</v>
-      </c>
-      <c r="C56" t="s">
-        <v>129</v>
+        <v>89</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="D56" t="s">
         <v>80</v>
@@ -1480,17 +1483,71 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
+        <v>131</v>
+      </c>
+      <c r="C57" t="s">
+        <v>128</v>
+      </c>
+      <c r="D57" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>132</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="D58" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D61" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>134</v>
+      </c>
+      <c r="C62" t="s">
+        <v>129</v>
+      </c>
+      <c r="D62" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
         <v>135</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="D57" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C60" s="4"/>
+      <c r="D63" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
basic jasper report added
</commit_message>
<xml_diff>
--- a/extra deatil/IMT Hub Initial Data Upload.xlsx
+++ b/extra deatil/IMT Hub Initial Data Upload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nabeel.jamil\Downloads\imrh\extra deatil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CD58B5-EC25-4B1F-B855-4CF1213BBA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9518C4E1-AD6B-4860-B90D-80A857D36871}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="141">
   <si>
     <t>ISO 2 Char</t>
   </si>
@@ -564,6 +564,9 @@
   </si>
   <si>
     <t>Fetch All Link Bank with Mito Partner</t>
+  </si>
+  <si>
+    <t>Api Detail for MTO Product</t>
   </si>
 </sst>
 </file>
@@ -964,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F940D0E-E75E-4A56-AAF4-E27BEE2B7AF5}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1544,6 +1547,14 @@
       </c>
       <c r="D63" t="s">
         <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>140</v>
+      </c>
+      <c r="B64" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">

</xml_diff>